<commit_message>
Add Simulcast Final Scedule
</commit_message>
<xml_diff>
--- a/70-534-2017 Two Room Schedule.xlsx
+++ b/70-534-2017 Two Room Schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="52">
   <si>
     <t>Speaker</t>
   </si>
@@ -229,6 +229,17 @@
   <si>
     <t>Presentation includes 15 min Lab and Q &amp; A</t>
   </si>
+  <si>
+    <t>What to Expect; Q&amp;A; Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluation Link: Please text MICROSOFT AZURE to 878787 to take part in a brief survey.  
+Survey Link:  http://t.validar.com/1/VBV7Q </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluation Link: Please text MICROSOFT AZURE to 878787 to take part in a brief survey.  
+Survey Link:  http://t.validar.com/1/VBV7Q  </t>
+  </si>
 </sst>
 </file>
 
@@ -238,7 +249,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +334,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -668,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -803,83 +821,86 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="20" fontId="2" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1206,7 +1227,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:D34"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1222,43 +1243,43 @@
   <sheetData>
     <row r="1" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B1" s="19"/>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B2" s="2"/>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50">
+      <c r="A3" s="59">
         <v>0.35416666666666669</v>
       </c>
       <c r="B3" s="21"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="53"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="51"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="17"/>
@@ -1295,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
@@ -1345,14 +1366,14 @@
       <c r="B9" s="24">
         <v>15</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="62" t="s">
+      <c r="D9" s="56"/>
+      <c r="E9" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="63"/>
+      <c r="F9" s="58"/>
     </row>
     <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.45">
       <c r="A10" s="17">
@@ -1401,14 +1422,14 @@
       <c r="B12" s="24">
         <v>60</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62" t="s">
+      <c r="D12" s="57"/>
+      <c r="E12" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="63"/>
+      <c r="F12" s="58"/>
     </row>
     <row r="13" spans="1:7" ht="46.8" x14ac:dyDescent="0.45">
       <c r="A13" s="17">
@@ -1459,14 +1480,14 @@
       <c r="B15" s="24">
         <v>40</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="62" t="s">
+      <c r="D15" s="56"/>
+      <c r="E15" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="63"/>
+      <c r="F15" s="58"/>
     </row>
     <row r="16" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="17">
@@ -1475,67 +1496,67 @@
       <c r="B16" s="24">
         <v>30</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60" t="s">
+      <c r="D16" s="52"/>
+      <c r="E16" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="61"/>
+      <c r="F16" s="54"/>
     </row>
     <row r="17" spans="1:6" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="16">
         <v>0.70833333333333337</v>
       </c>
       <c r="B17" s="22"/>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
     </row>
     <row r="19" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B19" s="2"/>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
     </row>
     <row r="20" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A20" s="50">
+      <c r="A20" s="59">
         <v>0.35416666666666669</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="51"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
     </row>
     <row r="22" spans="1:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="17"/>
@@ -1602,14 +1623,14 @@
       <c r="B25" s="24">
         <v>15</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="65"/>
-      <c r="E25" s="62" t="s">
+      <c r="D25" s="56"/>
+      <c r="E25" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="63"/>
+      <c r="F25" s="58"/>
     </row>
     <row r="26" spans="1:6" ht="46.8" x14ac:dyDescent="0.45">
       <c r="A26" s="17">
@@ -1638,14 +1659,14 @@
       <c r="B27" s="24">
         <v>60</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62" t="s">
+      <c r="D27" s="57"/>
+      <c r="E27" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="63"/>
+      <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A28" s="17">
@@ -1714,14 +1735,14 @@
       <c r="B31" s="24">
         <v>155</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="62" t="s">
+      <c r="D31" s="56"/>
+      <c r="E31" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="63"/>
+      <c r="F31" s="58"/>
     </row>
     <row r="32" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="17">
@@ -1730,50 +1751,37 @@
       <c r="B32" s="24">
         <v>30</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C32" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="59"/>
-      <c r="E32" s="60" t="s">
+      <c r="D32" s="52"/>
+      <c r="E32" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="61"/>
+      <c r="F32" s="54"/>
     </row>
     <row r="33" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="16">
         <v>0.70833333333333337</v>
       </c>
       <c r="B33" s="22"/>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
     </row>
     <row r="34" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C19:F19"/>
@@ -1790,6 +1798,19 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" location="syllabus-3"/>
@@ -1817,10 +1838,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,38 +1853,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
     </row>
     <row r="2" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
     </row>
     <row r="3" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="50">
+      <c r="A3" s="59">
         <v>0.35416666666666669</v>
       </c>
       <c r="B3" s="21"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="51"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="64"/>
     </row>
     <row r="5" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="17"/>
@@ -1926,10 +1947,10 @@
       <c r="B9" s="24">
         <v>15</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="67"/>
+      <c r="D9" s="68"/>
     </row>
     <row r="10" spans="1:4" ht="46.8" x14ac:dyDescent="0.45">
       <c r="A10" s="17">
@@ -1966,10 +1987,10 @@
       <c r="B12" s="24">
         <v>60</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:4" ht="46.8" x14ac:dyDescent="0.45">
       <c r="A13" s="17">
@@ -2006,10 +2027,10 @@
       <c r="B15" s="24">
         <v>40</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="67"/>
+      <c r="D15" s="68"/>
     </row>
     <row r="16" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="17">
@@ -2018,54 +2039,54 @@
       <c r="B16" s="24">
         <v>30</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="71"/>
     </row>
     <row r="17" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="16">
         <v>0.70833333333333337</v>
       </c>
       <c r="B17" s="22"/>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="64"/>
     </row>
     <row r="18" spans="1:4" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
     </row>
     <row r="20" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A20" s="50">
+      <c r="A20" s="59">
         <v>0.35416666666666669</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="52"/>
+      <c r="D20" s="61"/>
     </row>
     <row r="21" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="51"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="55"/>
+      <c r="D21" s="64"/>
     </row>
     <row r="22" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="17"/>
@@ -2114,10 +2135,10 @@
       <c r="B25" s="24">
         <v>15</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="67"/>
+      <c r="D25" s="68"/>
     </row>
     <row r="26" spans="1:4" ht="46.8" x14ac:dyDescent="0.45">
       <c r="A26" s="17">
@@ -2140,10 +2161,10 @@
       <c r="B27" s="24">
         <v>60</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="63"/>
+      <c r="D27" s="58"/>
     </row>
     <row r="28" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A28" s="17">
@@ -2194,10 +2215,10 @@
       <c r="B31" s="24">
         <v>155</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="67"/>
+      <c r="D31" s="68"/>
     </row>
     <row r="32" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="17">
@@ -2206,36 +2227,50 @@
       <c r="B32" s="24">
         <v>30</v>
       </c>
-      <c r="C32" s="68" t="s">
+      <c r="C32" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="69"/>
+      <c r="D32" s="71"/>
     </row>
     <row r="33" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="16">
         <v>0.70833333333333337</v>
       </c>
       <c r="B33" s="22"/>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="54"/>
+      <c r="D33" s="63"/>
     </row>
     <row r="34" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+    </row>
+    <row r="35" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="74"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C12:D12"/>
+  <mergeCells count="22">
+    <mergeCell ref="C35:D38"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:A4"/>
@@ -2247,6 +2282,11 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
@@ -2272,10 +2312,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2288,35 +2328,35 @@
   <sheetData>
     <row r="1" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B1" s="34"/>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="48"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B2" s="35"/>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="67"/>
     </row>
     <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50">
+      <c r="A3" s="59">
         <v>0.35416666666666669</v>
       </c>
       <c r="B3" s="21"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="51"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="64"/>
     </row>
     <row r="5" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="17"/>
@@ -2332,30 +2372,30 @@
     </row>
     <row r="6" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A6" s="17">
-        <v>0.375</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="B6" s="24">
         <v>10</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A7" s="17">
-        <v>0.38194444444444442</v>
+        <v>0.375</v>
       </c>
       <c r="B7" s="24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="46.8" x14ac:dyDescent="0.45">
@@ -2379,10 +2419,10 @@
       <c r="B9" s="24">
         <v>15</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="63"/>
+      <c r="D9" s="58"/>
     </row>
     <row r="10" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A10" s="17">
@@ -2419,10 +2459,10 @@
       <c r="B12" s="24">
         <v>60</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A13" s="17">
@@ -2459,10 +2499,10 @@
       <c r="B15" s="24">
         <v>40</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="58"/>
     </row>
     <row r="16" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="17">
@@ -2471,53 +2511,53 @@
       <c r="B16" s="24">
         <v>30</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="72"/>
+      <c r="D16" s="73"/>
     </row>
     <row r="17" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="16">
         <v>0.70833333333333337</v>
       </c>
       <c r="B17" s="22"/>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="54"/>
+      <c r="D17" s="63"/>
     </row>
     <row r="18" spans="1:4" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B19" s="35"/>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="49"/>
+      <c r="D19" s="67"/>
     </row>
     <row r="20" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A20" s="50">
+      <c r="A20" s="59">
         <v>0.35416666666666669</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="52"/>
+      <c r="D20" s="61"/>
     </row>
     <row r="21" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="51"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="55"/>
+      <c r="D21" s="64"/>
     </row>
     <row r="22" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="17"/>
@@ -2566,10 +2606,10 @@
       <c r="B25" s="24">
         <v>15</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="63"/>
+      <c r="D25" s="58"/>
     </row>
     <row r="26" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A26" s="17">
@@ -2592,10 +2632,10 @@
       <c r="B27" s="24">
         <v>60</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="63"/>
+      <c r="D27" s="58"/>
     </row>
     <row r="28" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A28" s="17">
@@ -2646,10 +2686,10 @@
       <c r="B31" s="24">
         <v>155</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="63"/>
+      <c r="D31" s="58"/>
     </row>
     <row r="32" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="17">
@@ -2658,31 +2698,55 @@
       <c r="B32" s="24">
         <v>30</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C32" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="72"/>
+      <c r="D32" s="73"/>
     </row>
     <row r="33" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="16">
         <v>0.70833333333333337</v>
       </c>
       <c r="B33" s="22"/>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="54"/>
+      <c r="D33" s="63"/>
     </row>
     <row r="34" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+    </row>
+    <row r="35" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="74"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="C35:D38"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C1:D1"/>
@@ -2699,11 +2763,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" location="syllabus-3"/>

</xml_diff>